<commit_message>
[Christopher] modulo carga masiva terminado, reporte de ganancias como módulo desde acceso permisos
</commit_message>
<xml_diff>
--- a/vistas/temp/plantilla.xlsx
+++ b/vistas/temp/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\peluqueria\vistas\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ABC177-2188-43E5-A630-87221B07B858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE862E-B87F-479A-BF5B-B15E0D3B86DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99FB7A3F-7D98-4F89-BBF3-76A5CBFBCDA6}"/>
   </bookViews>
@@ -155,7 +155,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-No debe superar los 50 caracteres.
+No debe superar los 20 caracteres.
 El código no debe repetirse.
 Por defecto, se colocará el último código del producto del local del usuario logeado.
 El código debe ser alfanumérico, combinando un prefijo en letras (ejemplo: "PRO", "ARP") y una secuencia numérica de 5 dígitos (ejemplo: "00001"), quedando el código así "PRO00001" o "ARP00020".</t>
@@ -914,17 +914,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2021,7 +2021,7 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,30 +2042,30 @@
   <sheetData>
     <row r="1" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="B1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
+      <c r="B1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
     </row>
     <row r="2" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -2212,20 +2212,20 @@
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26">
         <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>0</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="7">
@@ -2264,20 +2264,20 @@
     </row>
     <row r="5" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26">
         <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>0</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="7">
         <v>0</v>
       </c>
@@ -2314,20 +2314,20 @@
     </row>
     <row r="6" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26">
         <v>0</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>0</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="28"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="7">
         <v>0</v>
       </c>
@@ -2364,20 +2364,20 @@
     </row>
     <row r="7" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26">
         <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>0</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="7">
         <v>0</v>
       </c>
@@ -2414,20 +2414,20 @@
     </row>
     <row r="8" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26">
         <v>0</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>0</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="7">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
[Christopher] subo cambios corrección de errores en tickets y A4 de C/V/P
</commit_message>
<xml_diff>
--- a/vistas/temp/plantilla.xlsx
+++ b/vistas/temp/plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\peluqueria\vistas\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE862E-B87F-479A-BF5B-B15E0D3B86DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E6AA99-9D1D-47C6-A851-266D88CC25A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99FB7A3F-7D98-4F89-BBF3-76A5CBFBCDA6}"/>
   </bookViews>
@@ -530,12 +530,64 @@
     <t>COMENZAR A ESCRIBIR DESDE AQUÍ =&gt;</t>
   </si>
   <si>
+    <t>STOCK MIN.</t>
+  </si>
+  <si>
+    <t>FILA DE EJEMPLO (NO SE AGREGARÁ‎ ‎ ‎ ‎ ‎‎  
+EN LA BASE DE DATOS) =&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IDMEDIDA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IDLOCAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C. PRODUCTO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">NOMBRE DEL PRODUCTO </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -543,58 +595,6 @@
       </rPr>
       <t>*</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">C. PRODUCTO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>STOCK MIN.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">IDMEDIDA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">IDLOCAL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>FILA DE EJEMPLO (NO SE AGREGARÁ‎ ‎ ‎ ‎ ‎‎  
-EN LA BASE DE DATOS) =&gt;</t>
   </si>
 </sst>
 </file>
@@ -642,13 +642,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color indexed="81"/>
@@ -674,6 +667,13 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -902,7 +902,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -914,13 +914,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2020,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB844433-F2DA-4254-ABE6-C434F460947F}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,28 +2070,28 @@
     <row r="2" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="3" spans="1:23" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>1</v>

</xml_diff>